<commit_message>
bringing repo up to speed on testing
</commit_message>
<xml_diff>
--- a/Navigation/Test_cases_playground.xlsx
+++ b/Navigation/Test_cases_playground.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheil\OneDrive - PennO365\Documents\Robotics\SDE_Interview_Prep\Navigation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044D5DB0-E709-4574-9F13-3471EEAF3A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72AA342-5F4D-4733-9FFF-84B9FD3C433D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10980" yWindow="0" windowWidth="17820" windowHeight="16200" activeTab="2" xr2:uid="{144D234B-9EDF-4C60-BA78-862FC813572B}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="4" xr2:uid="{144D234B-9EDF-4C60-BA78-862FC813572B}"/>
   </bookViews>
   <sheets>
-    <sheet name="test_input" sheetId="1" r:id="rId1"/>
+    <sheet name="test_input_1" sheetId="1" r:id="rId1"/>
     <sheet name="test_input_2" sheetId="2" r:id="rId2"/>
     <sheet name="test_input_3" sheetId="3" r:id="rId3"/>
+    <sheet name="test_input_4" sheetId="5" r:id="rId4"/>
+    <sheet name="Time_Complexity" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="IQ_CH">110000</definedName>
@@ -317,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="24">
   <si>
     <t>#</t>
   </si>
@@ -360,12 +362,42 @@
   <si>
     <t xml:space="preserve"> [14 13 12 11 10  9  8  7  6  6  7  8  9 10 11 12 13 14]]</t>
   </si>
+  <si>
+    <t>test_input_1</t>
+  </si>
+  <si>
+    <t>test_input_2</t>
+  </si>
+  <si>
+    <t>test_input_3</t>
+  </si>
+  <si>
+    <t># of Avocados</t>
+  </si>
+  <si>
+    <t>Runtime (secs)</t>
+  </si>
+  <si>
+    <t>Held-Karp</t>
+  </si>
+  <si>
+    <t>Brute Force</t>
+  </si>
+  <si>
+    <t>test_input_4</t>
+  </si>
+  <si>
+    <t>2^n</t>
+  </si>
+  <si>
+    <t>n!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,13 +424,50 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u val="singleAccounting"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF062C53"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -428,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -436,11 +505,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="6"/>
@@ -516,6 +623,2579 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Time_Complexity!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Time_Complexity!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.372</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.131</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.303000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AEF1-4DAE-AEDC-A1A74BCD0A58}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2100951423"/>
+        <c:axId val="2100958623"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2100951423"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2100958623"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2100958623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2100951423"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Time_Complexity!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Time_Complexity!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.372</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.131</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.303000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D056-49CE-8731-5E8950E04163}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1996522543"/>
+        <c:axId val="1996520143"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1996522543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1996520143"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1996520143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1996522543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Time_Complexity!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Time_Complexity!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.372</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.131</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.303000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-600A-4E11-9B74-9D8F065B1DB6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1997021183"/>
+        <c:axId val="1997026463"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1997021183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1997026463"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1997026463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1997021183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -883,6 +3563,119 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D3FDFB4-E8EA-398F-D017-40FCB8DAA2EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>413558</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57842</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>108758</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>134042</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B3C03AD-E847-348D-1ABE-E9F7007B4386}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>372717</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>24019</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>41413</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>100219</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D244451-0FB6-747A-61F0-D1EDDC477D4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1621,10 +4414,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="@">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="@">
       <formula>NOT(ISERROR(SEARCH("@",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="#">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="#">
       <formula>NOT(ISERROR(SEARCH("#",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2069,10 +4862,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="@">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="@">
       <formula>NOT(ISERROR(SEARCH("@",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="#">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="#">
       <formula>NOT(ISERROR(SEARCH("#",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2087,7 +4880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79586CF0-040B-48B7-80AC-9E44AD526E0D}">
   <dimension ref="B3:Q15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="82" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="82" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2364,6 +5157,404 @@
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="@">
+      <formula>NOT(ISERROR(SEARCH("@",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="#">
+      <formula>NOT(ISERROR(SEARCH("#",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC095A7-A5B8-48A6-AD95-6CB9C2E01E90}">
+  <dimension ref="B3:Q17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="82" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="17" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
@@ -2377,4 +5568,135 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C98209-E298-4739-A7EC-F76912A257FC}">
+  <dimension ref="B2:H7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.372</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="G4" s="10">
+        <f>2^C4</f>
+        <v>32</v>
+      </c>
+      <c r="H4" s="10">
+        <f>+FACT(C4)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.131</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.159</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" ref="G5:G7" si="0">2^C5</f>
+        <v>32</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" ref="H5:H7" si="1">+FACT(C5)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3">
+        <v>13.303000000000001</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="G6" s="10">
+        <f t="shared" si="0"/>
+        <v>262144</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="1"/>
+        <v>6402373705728000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3">
+        <v>36</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="0"/>
+        <v>68719476736</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="1"/>
+        <v>3.7199332678990133E+41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <customProperties>
+    <customPr name="UniqueName" r:id="rId2"/>
+  </customProperties>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finishing touches on readme
</commit_message>
<xml_diff>
--- a/Navigation/Test_cases_playground.xlsx
+++ b/Navigation/Test_cases_playground.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheil\OneDrive - PennO365\Documents\Robotics\SDE_Interview_Prep\Navigation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F50ACD-2BEB-44F6-BA17-12AEEB94C7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58A7582-F769-43C1-86F8-35290C6EB902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="3" activeTab="5" xr2:uid="{144D234B-9EDF-4C60-BA78-862FC813572B}"/>
   </bookViews>
@@ -376,9 +376,6 @@
     <t># of Avocados</t>
   </si>
   <si>
-    <t>Held-Karp</t>
-  </si>
-  <si>
     <t>Brute Force</t>
   </si>
   <si>
@@ -435,14 +432,17 @@
   <si>
     <t>Test Case</t>
   </si>
+  <si>
+    <t>DP Solution</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="#,##0_);\(#,##0\);#,##0_);@_)"/>
-    <numFmt numFmtId="169" formatCode=";;;"/>
+    <numFmt numFmtId="164" formatCode="#,##0_);\(#,##0\);#,##0_);@_)"/>
+    <numFmt numFmtId="166" formatCode="0.E+00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -568,16 +568,16 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,10 +725,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.5538763228184068E-2"/>
-          <c:y val="9.8644895860118278E-2"/>
-          <c:w val="0.86070458544847428"/>
-          <c:h val="0.78271975902729307"/>
+          <c:x val="0.14684449781245473"/>
+          <c:y val="0.17328766116886454"/>
+          <c:w val="0.72807881818622056"/>
+          <c:h val="0.63809940124159714"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -738,7 +738,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Held-Karp Implementation</c:v>
+            <c:v>Dynamic Programming Soln</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -901,7 +901,7 @@
             <c:numRef>
               <c:f>Time_Complexity!$E$4:$E$12</c:f>
               <c:numCache>
-                <c:formatCode>;;;</c:formatCode>
+                <c:formatCode>0.E+00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>32</c:v>
@@ -959,6 +959,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># of Avocados</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1002,6 +1051,60 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000"/>
+                  <a:t>DP</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" baseline="0"/>
+                  <a:t> Solution Runtime (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0_);\(#,##0\);#,##0_);@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1046,7 +1149,56 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
-        <c:numFmt formatCode=";;;" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="800"/>
+                  <a:t>y=2^n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1065,7 +1217,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="700" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -1093,6 +1245,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="773804751"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1111,8 +1264,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.0000040250065603E-2"/>
-          <c:y val="9.3303456635932848E-3"/>
+          <c:x val="5.0000149179501276E-2"/>
+          <c:y val="2.7991036990779854E-2"/>
           <c:w val="0.89999993114792254"/>
           <c:h val="8.4752231568893943E-2"/>
         </c:manualLayout>
@@ -4004,7 +4157,7 @@
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>21</v>
@@ -4015,17 +4168,17 @@
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -4357,7 +4510,7 @@
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10">
         <v>19</v>
@@ -4365,42 +4518,42 @@
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -4424,7 +4577,7 @@
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4438,17 +4591,17 @@
   <sheetData>
     <row r="2" spans="2:7" ht="17.25" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="G2" s="6"/>
     </row>
@@ -4456,16 +4609,16 @@
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -4478,13 +4631,13 @@
       <c r="D4" s="12">
         <v>0.13</v>
       </c>
-      <c r="E4" s="13">
-        <f>2^C4</f>
+      <c r="E4" s="14">
+        <f t="shared" ref="E4:E12" si="0">2^C4</f>
         <v>32</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="10">
-        <f>+FACT(C4)</f>
+        <f t="shared" ref="G4:G10" si="1">+FACT(C4)</f>
         <v>120</v>
       </c>
     </row>
@@ -4498,13 +4651,13 @@
       <c r="D5" s="12">
         <v>1.1339999999999999</v>
       </c>
-      <c r="E5" s="13">
-        <f>2^C5</f>
+      <c r="E5" s="14">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="10">
-        <f>+FACT(C5)</f>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
     </row>
@@ -4513,13 +4666,13 @@
         <v>8</v>
       </c>
       <c r="D6" s="12"/>
-      <c r="E6" s="13">
-        <f>2^C6</f>
+      <c r="E6" s="14">
+        <f t="shared" si="0"/>
         <v>256</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="10">
-        <f>+FACT(C6)</f>
+        <f t="shared" si="1"/>
         <v>40320</v>
       </c>
     </row>
@@ -4528,13 +4681,13 @@
         <v>10</v>
       </c>
       <c r="D7" s="12"/>
-      <c r="E7" s="13">
-        <f>2^C7</f>
+      <c r="E7" s="14">
+        <f t="shared" si="0"/>
         <v>1024</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="10">
-        <f>+FACT(C7)</f>
+        <f t="shared" si="1"/>
         <v>3628800</v>
       </c>
     </row>
@@ -4543,13 +4696,13 @@
         <v>12</v>
       </c>
       <c r="D8" s="12"/>
-      <c r="E8" s="13">
-        <f>2^C8</f>
+      <c r="E8" s="14">
+        <f t="shared" si="0"/>
         <v>4096</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="10">
-        <f>+FACT(C8)</f>
+        <f t="shared" si="1"/>
         <v>479001600</v>
       </c>
     </row>
@@ -4558,13 +4711,13 @@
         <v>16</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" s="13">
-        <f>2^C9</f>
+      <c r="E9" s="14">
+        <f t="shared" si="0"/>
         <v>65536</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="10">
-        <f>+FACT(C9)</f>
+        <f t="shared" si="1"/>
         <v>20922789888000</v>
       </c>
     </row>
@@ -4578,19 +4731,19 @@
       <c r="D10" s="12">
         <v>14.199</v>
       </c>
-      <c r="E10" s="13">
-        <f>2^C10</f>
+      <c r="E10" s="14">
+        <f t="shared" si="0"/>
         <v>262144</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="10">
-        <f>+FACT(C10)</f>
+        <f t="shared" si="1"/>
         <v>6402373705728000</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3">
         <v>19</v>
@@ -4598,18 +4751,18 @@
       <c r="D11" s="12">
         <v>33.843000000000004</v>
       </c>
-      <c r="E11" s="13">
-        <f>2^C11</f>
+      <c r="E11" s="14">
+        <f t="shared" si="0"/>
         <v>524288</v>
       </c>
       <c r="G11" s="10">
-        <f t="shared" ref="G11" si="0">+FACT(C11)</f>
+        <f t="shared" ref="G11" si="2">+FACT(C11)</f>
         <v>1.21645100408832E+17</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3">
         <v>21</v>
@@ -4618,8 +4771,8 @@
         <f>2*60+53.068</f>
         <v>173.06799999999998</v>
       </c>
-      <c r="E12" s="13">
-        <f>2^C12</f>
+      <c r="E12" s="14">
+        <f t="shared" si="0"/>
         <v>2097152</v>
       </c>
       <c r="G12" s="10">

</xml_diff>